<commit_message>
Dec 16 201216 dpsv2 test version
</commit_message>
<xml_diff>
--- a/resources/customdata/specialtags.xlsx
+++ b/resources/customdata/specialtags.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$22</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
   <si>
     <t>tag</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -814,42 +814,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>%f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>表示在</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Monaco"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">state.options.ranged_penalty == true </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>时，atk_scale需要乘算的倍率（hard coded）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[%s, %s…] / true</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -890,14 +854,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>%d / "all"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>指定最大目标数，all为全打</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>sec</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -962,6 +918,34 @@
       </rPr>
       <t>攻击间隔相关，需要延后计算</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表示该buff的倍率为距离惩罚倍率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no_ranged_penalty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表示该buff无视ranged_penalty倍率标签</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%d / "aoe" / "block"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指定最大目标数，aoe为全打，block为阻挡数（阻挡数改变时不要用）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1061,7 +1045,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1073,6 +1057,8 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1353,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.875" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1457,13 +1443,13 @@
     </row>
     <row r="9" spans="1:3" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1515,135 +1501,143 @@
         <v>56</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+    <row r="18" spans="1:3" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
+    <row r="19" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>48</v>
+      <c r="B19" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
     <row r="22" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
-        <v>18</v>
+      <c r="A22" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>50</v>
+        <v>62</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="5"/>
     </row>
     <row r="27" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
@@ -1726,8 +1720,11 @@
     <row r="53" spans="1:1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5"/>
     </row>
+    <row r="54" spans="1:1" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="5"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C21">
+  <autoFilter ref="A1:C22">
     <sortState ref="A2:C25">
       <sortCondition ref="A1:A21"/>
     </sortState>

</xml_diff>